<commit_message>
updated ready for final!
</commit_message>
<xml_diff>
--- a/Parameters.xlsx
+++ b/Parameters.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17426"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JC\Documents\GitHub\OptimTurf\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="30" windowWidth="20115" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="36" windowWidth="20112" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -30,7 +35,7 @@
     <definedName name="solver_typ" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_val" localSheetId="0" hidden="1">0</definedName>
   </definedNames>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
@@ -55,17 +60,20 @@
     <t>N2011</t>
   </si>
   <si>
-    <t>N</t>
+    <t>SlnSSQ</t>
   </si>
   <si>
-    <t>SlnSSQ</t>
+    <t>Observed</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="168" formatCode="0.0000"/>
+  </numFmts>
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -94,25 +102,46 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="es-MX"/>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
         <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -122,7 +151,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>N</c:v>
+                  <c:v>Observed</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -141,10 +170,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Hoja1!$A$9:$A$19</c:f>
+              <c:f>Hoja1!$A$9:$A$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>2011</c:v>
                 </c:pt>
@@ -168,25 +197,16 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>2018</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>2019</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>2020</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>2021</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Hoja1!$B$9:$B$19</c:f>
+              <c:f>Hoja1!$B$9:$B$16</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:formatCode>0.0000</c:formatCode>
+                <c:ptCount val="8"/>
                 <c:pt idx="1">
                   <c:v>0.41176469999999998</c:v>
                 </c:pt>
@@ -206,6 +226,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-9977-4AC1-98AA-10F3FB3B3A10}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -233,10 +258,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Hoja1!$A$9:$A$19</c:f>
+              <c:f>Hoja1!$A$9:$A$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>2011</c:v>
                 </c:pt>
@@ -260,25 +285,16 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>2018</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>2019</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>2020</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>2021</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Hoja1!$C$9:$C$19</c:f>
+              <c:f>Hoja1!$C$9:$C$16</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:formatCode>0.0000</c:formatCode>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>0.20001020602974909</c:v>
                 </c:pt>
@@ -302,21 +318,25 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>3.1927383530155602</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>3.1929934466761609</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>3.1929721752609521</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>3.1929739507015094</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-9977-4AC1-98AA-10F3FB3B3A10}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
         <c:axId val="146579456"/>
         <c:axId val="146569472"/>
       </c:scatterChart>
@@ -325,9 +345,43 @@
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-MX"/>
+                  <a:t>Years</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="dk1">
+                <a:shade val="95000"/>
+                <a:satMod val="105000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:prstDash val="solid"/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
         <c:crossAx val="146569472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
@@ -337,21 +391,90 @@
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
-        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-MX"/>
+                  <a:t>Density </a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="es-MX" sz="1000" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>(orgs 60m</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="es-MX" sz="1000" b="0" i="0" u="none" strike="noStrike" baseline="30000">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>-1</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="es-MX" sz="1000" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>)</a:t>
+                </a:r>
+                <a:endParaRPr lang="es-MX"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="dk1">
+                <a:shade val="95000"/>
+                <a:satMod val="105000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:prstDash val="solid"/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
         <c:crossAx val="146579456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout/>
+      <c:legendPos val="t"/>
+      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
+  <c:spPr>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr b="0"/>
+      </a:pPr>
+      <a:endParaRPr lang="es-MX"/>
+    </a:p>
+  </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
@@ -377,7 +500,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="1 Gráfico"/>
+        <xdr:cNvPr id="2" name="1 Gráfico">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -396,7 +525,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -438,7 +567,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -470,9 +599,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -504,6 +651,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -679,16 +844,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="P4" sqref="P4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -704,7 +869,7 @@
         <v>53216.230232308619</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -712,7 +877,7 @@
         <v>1.0834599230819744</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -720,21 +885,21 @@
         <v>0.20001020602974909</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B5">
         <f>SUM(D9:D14)</f>
         <v>2.5155987980824253E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C8" t="s">
         <v>4</v>
@@ -743,254 +908,255 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>2011</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="1">
         <f>B3</f>
         <v>0.20001020602974909</v>
       </c>
-      <c r="D9" t="str">
+      <c r="D9" s="1" t="str">
         <f>IF(B9=0,"",(LN(C9)-LN(B9))^2)</f>
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>2012</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="1">
         <v>0.41176469999999998</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="1">
         <f>C9+($B$2*C9*(1-(C9/$B$1)))</f>
         <v>0.40313881200719837</v>
       </c>
-      <c r="D10">
-        <f t="shared" ref="D10:D24" si="0">IF(B10=0,"",(LN(C10)-LN(B10))^2)</f>
+      <c r="D10" s="1">
+        <f>IF(B10=0,"",(LN(C10)-LN(B10))^2)</f>
         <v>4.4821633852493159E-4</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>2013</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="1">
         <v>0.73333329999999997</v>
       </c>
-      <c r="C11">
-        <f t="shared" ref="C11:C24" si="1">C10+($B$2*C10*(1-(C10/$B$1)))</f>
+      <c r="C11" s="1">
+        <f t="shared" ref="C11:C24" si="0">C10+($B$2*C10*(1-(C10/$B$1)))</f>
         <v>0.7847759454139287</v>
       </c>
-      <c r="D11">
-        <f t="shared" si="0"/>
+      <c r="D11" s="1">
+        <f t="shared" ref="D10:D24" si="1">IF(B11=0,"",(LN(C11)-LN(B11))^2)</f>
         <v>4.596562290484457E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>2014</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="1">
         <v>1.5945946</v>
       </c>
-      <c r="C12">
-        <f t="shared" si="1"/>
+      <c r="C12" s="1">
+        <f t="shared" si="0"/>
         <v>1.4260672409318875</v>
       </c>
-      <c r="D12">
-        <f t="shared" si="0"/>
+      <c r="D12" s="1">
+        <f t="shared" si="1"/>
         <v>1.2476680058999814E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>2015</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="1">
         <v>2.0975609999999998</v>
       </c>
-      <c r="C13">
-        <f t="shared" si="1"/>
+      <c r="C13" s="1">
+        <f t="shared" si="0"/>
         <v>2.2810770251582002</v>
       </c>
-      <c r="D13">
-        <f t="shared" si="0"/>
+      <c r="D13" s="1">
+        <f t="shared" si="1"/>
         <v>7.0345911750103341E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>2016</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="1">
         <v>3.0609755999999999</v>
       </c>
-      <c r="C14">
-        <f t="shared" si="1"/>
+      <c r="C14" s="1">
+        <f t="shared" si="0"/>
         <v>2.9869119302487608</v>
       </c>
-      <c r="D14">
-        <f t="shared" si="0"/>
+      <c r="D14" s="1">
+        <f t="shared" si="1"/>
         <v>5.999381178047184E-4</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>2017</v>
       </c>
-      <c r="C15">
-        <f t="shared" si="1"/>
+      <c r="C15" s="1">
+        <f t="shared" si="0"/>
         <v>3.1957634201381944</v>
       </c>
-      <c r="D15" t="str">
-        <f t="shared" si="0"/>
+      <c r="D15" s="1" t="str">
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>2018</v>
       </c>
-      <c r="C16">
-        <f t="shared" si="1"/>
+      <c r="C16" s="1">
+        <f t="shared" si="0"/>
         <v>3.1927383530155602</v>
       </c>
-      <c r="D16" t="str">
-        <f t="shared" si="0"/>
+      <c r="D16" s="1" t="str">
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>2019</v>
       </c>
-      <c r="C17">
-        <f t="shared" si="1"/>
+      <c r="C17" s="1">
+        <f t="shared" si="0"/>
         <v>3.1929934466761609</v>
       </c>
-      <c r="D17" t="str">
-        <f t="shared" si="0"/>
+      <c r="D17" s="1" t="str">
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>2020</v>
       </c>
-      <c r="C18">
-        <f t="shared" si="1"/>
+      <c r="C18" s="1">
+        <f t="shared" si="0"/>
         <v>3.1929721752609521</v>
       </c>
-      <c r="D18" t="str">
-        <f t="shared" si="0"/>
+      <c r="D18" s="1" t="str">
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>2021</v>
       </c>
-      <c r="C19">
-        <f t="shared" si="1"/>
+      <c r="C19" s="1">
+        <f t="shared" si="0"/>
         <v>3.1929739507015094</v>
       </c>
-      <c r="D19" t="str">
-        <f t="shared" si="0"/>
+      <c r="D19" s="1" t="str">
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>2022</v>
       </c>
-      <c r="C20">
-        <f t="shared" si="1"/>
+      <c r="C20" s="1">
+        <f t="shared" si="0"/>
         <v>3.1929738025242824</v>
       </c>
-      <c r="D20" t="str">
-        <f t="shared" si="0"/>
+      <c r="D20" s="1" t="str">
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>2023</v>
       </c>
-      <c r="C21">
-        <f t="shared" si="1"/>
+      <c r="C21" s="1">
+        <f t="shared" si="0"/>
         <v>3.1929738148911486</v>
       </c>
-      <c r="D21" t="str">
-        <f t="shared" si="0"/>
+      <c r="D21" s="1" t="str">
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>2024</v>
       </c>
-      <c r="C22">
-        <f t="shared" si="1"/>
+      <c r="C22" s="1">
+        <f t="shared" si="0"/>
         <v>3.1929738138590107</v>
       </c>
-      <c r="D22" t="str">
-        <f t="shared" si="0"/>
+      <c r="D22" s="1" t="str">
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>2025</v>
       </c>
-      <c r="C23">
-        <f t="shared" si="1"/>
+      <c r="C23" s="1">
+        <f t="shared" si="0"/>
         <v>3.1929738139451529</v>
       </c>
-      <c r="D23" t="str">
-        <f t="shared" si="0"/>
+      <c r="D23" s="1" t="str">
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>2026</v>
       </c>
-      <c r="C24">
-        <f t="shared" si="1"/>
+      <c r="C24" s="1">
+        <f t="shared" si="0"/>
         <v>3.1929738139379635</v>
       </c>
-      <c r="D24" t="str">
-        <f t="shared" si="0"/>
+      <c r="D24" s="1" t="str">
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>